<commit_message>
pause for reserach nodejs
</commit_message>
<xml_diff>
--- a/csharpNote.xlsx
+++ b/csharpNote.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="ASPMVC" sheetId="3" r:id="rId4"/>
     <sheet name="ASPCoreAndAngula" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>https://jsonutils.com/</t>
   </si>
@@ -310,12 +310,18 @@
   <si>
     <t>https://www.npmjs.com/package/time-ago-pipe</t>
   </si>
+  <si>
+    <t>https://cli.angular.io/</t>
+  </si>
+  <si>
+    <t>angular cli</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,199 +421,6 @@
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Control 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Control 4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -651,7 +464,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,10 +496,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -718,7 +530,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -894,41 +705,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -940,41 +751,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -985,16 +796,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1006,71 +817,71 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8">
       <c r="C3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8">
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8">
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8">
       <c r="C6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8">
       <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8">
       <c r="C10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8">
       <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8">
       <c r="C12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8">
       <c r="C13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8">
       <c r="H14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8">
       <c r="H15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28" t="s">
         <v>23</v>
       </c>
@@ -1081,21 +892,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1106,7 +917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="I4" t="s">
         <v>49</v>
       </c>
@@ -1114,7 +925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1122,7 +933,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
+      <c r="K8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="K10" t="s">
         <v>54</v>
       </c>
@@ -1133,7 +952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1144,7 +963,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1155,7 +974,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1166,17 +985,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1187,22 +1006,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1218,7 +1037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="43.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1232,7 +1051,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1249,10 +1068,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="S24" s="6"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1266,7 +1085,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1275,7 +1094,7 @@
       </c>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -1286,7 +1105,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1295,7 +1114,7 @@
       </c>
       <c r="S28" s="6"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="S29" s="6" t="s">
         <v>72</v>
       </c>
@@ -1303,20 +1122,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="S30" s="6"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="L32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="L34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1331,109 +1150,12 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId4"/>
   <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="Control 1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId8" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId8" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId10" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId10" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId12" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId12" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <control shapeId="1028" r:id="rId5" name="Control 4"/>
+    <control shapeId="1027" r:id="rId6" name="Control 3"/>
+    <control shapeId="1026" r:id="rId7" name="Control 2"/>
+    <control shapeId="1025" r:id="rId8" name="Control 1"/>
   </controls>
 </worksheet>
 </file>
</xml_diff>